<commit_message>
GameEnter 응답 추가 (PlayerPacket)
</commit_message>
<xml_diff>
--- a/Data/Excel/Model/User/KingdomMap.xlsx
+++ b/Data/Excel/Model/User/KingdomMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitWorks\GameServerStudyAspNet\Data\Excel\Model\User\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE1E873-1723-4339-9DD7-E4D7D341F7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD24AC0-04D4-41B0-AF41-853846505314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{B14C0FCD-ADAC-43B5-88EF-CD027C78C01B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B14C0FCD-ADAC-43B5-88EF-CD027C78C01B}"/>
   </bookViews>
   <sheets>
     <sheet name="Packet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
@@ -74,14 +74,27 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>XSize</t>
-  </si>
-  <si>
-    <t>Ysize</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>INT</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>PlacedKingdomItemList</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>LIST:PlacedKingdomItemPacket</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Packet</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SizeY</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SizeX</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1016,10 +1029,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCC6768-C9E8-4795-B55A-C1C942DE1B76}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1065,18 +1078,18 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1086,6 +1099,9 @@
       <c r="B5" t="s">
         <v>12</v>
       </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1093,6 +1109,17 @@
       </c>
       <c r="B6" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>